<commit_message>
working on new filter
</commit_message>
<xml_diff>
--- a/Kunden-Data.xlsx
+++ b/Kunden-Data.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="28455" windowHeight="12540"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="28455" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kunden-Data" sheetId="1" r:id="rId1"/>
+    <sheet name="SHEET 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>VP-Name</t>
   </si>
@@ -116,13 +117,25 @@
   <si>
     <t>ahmadkuedr@gmail.com</t>
   </si>
+  <si>
+    <t>hj</t>
+  </si>
+  <si>
+    <t>kjh</t>
+  </si>
+  <si>
+    <t>jkh</t>
+  </si>
+  <si>
+    <t>jh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -616,7 +629,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -965,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8144,4 +8157,47 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>897</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>897</v>
+      </c>
+      <c r="D2">
+        <v>897</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>